<commit_message>
change DPV spreadsheets to new schema
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/base.xlsx
+++ b/documentation-generator/vocab_csv/base.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="321">
   <si>
     <t>preffix</t>
   </si>
@@ -631,7 +631,7 @@
     <t>Resolution</t>
   </si>
   <si>
-    <t>PersonalDataHandling</t>
+    <t>dpv:PersonalDataHandling</t>
   </si>
   <si>
     <t>Personal Data Handling</t>
@@ -655,7 +655,7 @@
     <t>https://www.w3.org/2019/04/05-dpvcg-minutes.html</t>
   </si>
   <si>
-    <t>PersonalData</t>
+    <t>dpv:PersonalData</t>
   </si>
   <si>
     <t>Personal Data</t>
@@ -698,6 +698,9 @@
     <t>https://www.w3.org/community/dpvcg/wiki/MinutesOfMeeting_20220119</t>
   </si>
   <si>
+    <t>dpv:Processing</t>
+  </si>
+  <si>
     <t>Processing</t>
   </si>
   <si>
@@ -720,6 +723,9 @@
     </r>
   </si>
   <si>
+    <t>dpv:Purpose</t>
+  </si>
+  <si>
     <t>Purpose</t>
   </si>
   <si>
@@ -730,6 +736,9 @@
   </si>
   <si>
     <t>(SPECIAL Project,https://specialprivacy.ercim.eu/)</t>
+  </si>
+  <si>
+    <t>dpv:Recipient</t>
   </si>
   <si>
     <t>Recipient</t>
@@ -760,7 +769,7 @@
     </r>
   </si>
   <si>
-    <t>TechnicalOrganisationalMeasure</t>
+    <t>dpv:TechnicalOrganisationalMeasure</t>
   </si>
   <si>
     <t>Technical and Organisational Measure</t>
@@ -772,7 +781,7 @@
     <t>Bud Bruegger</t>
   </si>
   <si>
-    <t>LegalBasis</t>
+    <t>dpv:LegalBasis</t>
   </si>
   <si>
     <t>Legal Basis</t>
@@ -784,7 +793,7 @@
     <t>Legal basis (plural: legal bases) are defined by legislations and regulations, whose applicability is usually restricted to specific jurisdictions.</t>
   </si>
   <si>
-    <t>DataSubject</t>
+    <t>dpv:DataSubject</t>
   </si>
   <si>
     <t>Data Subject</t>
@@ -799,7 +808,7 @@
     <t>(GDPR Art.4-1g,https://eur-lex.europa.eu/eli/reg/2016/679/art_4/par_1/oj)</t>
   </si>
   <si>
-    <t>DataController</t>
+    <t>dpv:DataController</t>
   </si>
   <si>
     <t>Data Controller</t>
@@ -814,6 +823,9 @@
     <t>(GDPR Art.4-7g,https://eur-lex.europa.eu/eli/reg/2016/679/art_4/par_7/oj)</t>
   </si>
   <si>
+    <t>dpv:Right</t>
+  </si>
+  <si>
     <t>Right</t>
   </si>
   <si>
@@ -829,7 +841,7 @@
     <t>https://www.w3.org/2020/11/18-dpvcg-minutes.html</t>
   </si>
   <si>
-    <t>DataSubjectRight</t>
+    <t>dpv:DataSubjectRight</t>
   </si>
   <si>
     <t>Data Subject Right</t>
@@ -838,13 +850,13 @@
     <t>The rights applicable or provided to a Data Subject</t>
   </si>
   <si>
-    <t>dpv:Right</t>
-  </si>
-  <si>
     <t>Based on use of definitions, the notion of 'Data Subject Right' can be equivalent to 'Individual Right' or 'Right of a Person'</t>
   </si>
   <si>
     <t>Beatriz Esteves, Georg P Krog, Harshvardhan Pandit</t>
+  </si>
+  <si>
+    <t>dpv:Risk</t>
   </si>
   <si>
     <t>Risk</t>
@@ -3214,10 +3226,10 @@
         <v>224</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>208</v>
@@ -3227,14 +3239,14 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>219</v>
       </c>
       <c r="I4" s="34"/>
       <c r="J4" s="13" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K4" s="8">
         <v>43560.0</v>
@@ -3271,13 +3283,13 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>208</v>
@@ -3287,14 +3299,14 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>219</v>
       </c>
       <c r="I5" s="34"/>
       <c r="J5" s="6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="K5" s="8">
         <v>43560.0</v>
@@ -3331,32 +3343,32 @@
     </row>
     <row r="6">
       <c r="A6" s="38" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>217</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>219</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="K6" s="8">
         <v>43560.0</v>
@@ -3393,13 +3405,13 @@
     </row>
     <row r="7">
       <c r="A7" s="38" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>208</v>
@@ -3422,7 +3434,7 @@
         <v>210</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>212</v>
@@ -3447,13 +3459,13 @@
     </row>
     <row r="8">
       <c r="A8" s="38" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>208</v>
@@ -3465,7 +3477,7 @@
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
       <c r="I8" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="8">
@@ -3501,16 +3513,16 @@
     </row>
     <row r="9">
       <c r="A9" s="38" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>217</v>
@@ -3519,10 +3531,10 @@
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
       <c r="I9" s="6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K9" s="8">
         <v>43560.0</v>
@@ -3559,16 +3571,16 @@
     </row>
     <row r="10">
       <c r="A10" s="38" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>217</v>
@@ -3577,10 +3589,10 @@
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
       <c r="I10" s="6" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="K10" s="8">
         <v>43560.0</v>
@@ -3617,13 +3629,13 @@
     </row>
     <row r="11">
       <c r="A11" s="42" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>208</v>
@@ -3635,7 +3647,7 @@
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="42" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="J11" s="42"/>
       <c r="K11" s="45">
@@ -3646,10 +3658,10 @@
         <v>210</v>
       </c>
       <c r="N11" s="42" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="P11" s="44"/>
       <c r="Q11" s="44"/>
@@ -3671,16 +3683,16 @@
     </row>
     <row r="12">
       <c r="A12" s="42" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E12" s="42" t="s">
         <v>217</v>
@@ -3689,7 +3701,7 @@
       <c r="G12" s="44"/>
       <c r="H12" s="44"/>
       <c r="I12" s="42" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="J12" s="42"/>
       <c r="K12" s="45">
@@ -3700,10 +3712,10 @@
         <v>210</v>
       </c>
       <c r="N12" s="42" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="O12" s="46" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
@@ -3724,14 +3736,14 @@
       <c r="AF12" s="44"/>
     </row>
     <row r="13">
-      <c r="A13" s="47" t="s">
-        <v>267</v>
+      <c r="A13" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>208</v>
@@ -3743,7 +3755,7 @@
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
       <c r="I13" s="6" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="8">
@@ -3754,10 +3766,10 @@
         <v>210</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="O13" s="41" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
@@ -6765,13 +6777,13 @@
         <v>192</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="G1" s="27" t="s">
         <v>196</v>
@@ -6803,22 +6815,22 @@
     </row>
     <row r="2">
       <c r="A2" s="38" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>208</v>
       </c>
       <c r="E2" s="38" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
@@ -6834,7 +6846,7 @@
         <v>210</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>212</v>
@@ -6855,13 +6867,13 @@
     </row>
     <row r="3">
       <c r="A3" s="38" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>208</v>
@@ -6871,7 +6883,7 @@
         <v>dpv:DataSubject</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
@@ -6887,7 +6899,7 @@
         <v>210</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>212</v>
@@ -6908,13 +6920,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>208</v>
@@ -6924,7 +6936,7 @@
         <v>dpv:LegalBasis</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
@@ -6961,13 +6973,13 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>208</v>
@@ -6977,7 +6989,7 @@
         <v>dpv:PersonalData</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
@@ -6991,7 +7003,7 @@
         <v>210</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="O5" s="41" t="s">
         <v>223</v>
@@ -7012,13 +7024,13 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>208</v>
@@ -7028,7 +7040,7 @@
         <v>dpv:PersonalDataHandling</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
@@ -7042,7 +7054,7 @@
         <v>210</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>223</v>
@@ -7063,13 +7075,13 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>208</v>
@@ -7079,13 +7091,13 @@
         <v>dpv:Processing</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
       <c r="J7" s="6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="K7" s="8">
         <v>43559.0</v>
@@ -7097,7 +7109,7 @@
         <v>210</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>212</v>
@@ -7118,13 +7130,13 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>208</v>
@@ -7134,13 +7146,13 @@
         <v>dpv:Purpose</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="K8" s="8">
         <v>43559.0</v>
@@ -7152,7 +7164,7 @@
         <v>210</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="O8" s="9" t="s">
         <v>212</v>
@@ -7173,13 +7185,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>208</v>
@@ -7189,13 +7201,13 @@
         <v>dpv:Recipient</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="K9" s="8">
         <v>43559.0</v>
@@ -7207,7 +7219,7 @@
         <v>210</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="O9" s="9" t="s">
         <v>212</v>
@@ -7228,13 +7240,13 @@
     </row>
     <row r="10">
       <c r="A10" s="42" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>208</v>
@@ -7244,7 +7256,7 @@
         <v>dpv:Right</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G10" s="44"/>
       <c r="H10" s="44"/>
@@ -7258,10 +7270,10 @@
         <v>210</v>
       </c>
       <c r="N10" s="42" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="O10" s="46" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
@@ -7279,13 +7291,13 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>208</v>
@@ -7295,7 +7307,7 @@
         <v>dpv:Risk</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -7309,10 +7321,10 @@
         <v>210</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
@@ -7330,13 +7342,13 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>208</v>
@@ -7346,7 +7358,7 @@
         <v>dpv:TechnicalOrganisationalMeasure</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
@@ -7362,7 +7374,7 @@
         <v>210</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="O12" s="9" t="s">
         <v>212</v>
@@ -7389,43 +7401,43 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C15" s="48"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C16" s="48"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C17" s="48"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C18" s="48"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C19" s="48"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C20" s="48"/>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C21" s="48"/>
     </row>

</xml_diff>